<commit_message>
[ :sparkles: | #18 ] 수정사항 수정
</commit_message>
<xml_diff>
--- a/src/assets/data/info.xlsx
+++ b/src/assets/data/info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/win-air/Documents/Study/47th-web/src/assets/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/win-air/Documents/GitHub/47th-web/src/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6995C2-DFF0-2F4B-A3B6-9A142C0B8893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3D6362-5BD0-104C-94AB-ADB43CAFB0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36260" yWindow="11980" windowWidth="34200" windowHeight="21100" xr2:uid="{F526FC34-6726-9340-9C7C-462111DE0477}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="17100" windowHeight="21360" xr2:uid="{F526FC34-6726-9340-9C7C-462111DE0477}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -550,100 +550,97 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>src/assets/images/webp/1봄_42기_김성근_전자재료공학과.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/1봄_45기_경준하_경영학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/1봄_45기_황서진_컴퓨터정보공학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/1봄_46기_김가영_미디어커뮤니케이션학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/1봄_46기_이재명_미디어커뮤니케이션.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/2여름_42기_김성근_전자재료공학과.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/2여름_42기_변지욱_미디어커뮤니케이션학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/2여름_43기_박하민_건축공학과.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/2여름_43기_신해원_경영학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/2여름_44기_곽철우_정보융합학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/2여름_45기_안예원_국제통상학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/2여름_46기_박예서_전자공학과.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/2여름_46기_배중근_국제학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/2여름_46기_이찬영_국제통상학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/2여름_46기_정성호_동북아문화산업학부.webp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/assets/images/webp/3가을_41기_이민우_화학과.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/3가을_45기_안세은_미디어커뮤니케이션학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/3가을_46기_강민서_전자공학과.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/3가을_46기_박지원_동북아문화산업학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/3가을_46기_방여원_경영학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/3가을_46기_송희수_정보융합학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/3가을_46기_윤영수_미디어커뮤니케이션.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/4겨울_41기_홍자형_스포츠융합과학과.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/4겨울_42기_백채원_영어산업학과.webp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/assets/images/webp/4겨울_42기_최승아_컴정공.webp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/assets/images/webp/4겨울_44기_이가영_미디어커뮤니케이션학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/4겨울_44기_이아란_정보융합학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/4겨울_46기_김유민_정보융합학부.webp</t>
-  </si>
-  <si>
-    <t>src/assets/images/webp/4겨울_46기_유용규_국제학부.webp</t>
-  </si>
-  <si>
     <t>가을 햇살이 조용히 비추는 골목길. 나뭇잎이 이따금 떨어지는 모습은 가을의 끝자락을 암시한다. 이 골목은 계절이 남긴 발자국처럼, 사라져가는 가을을 간직한 채 머물러 있다.</t>
   </si>
   <si>
     <t xml:space="preserve">끝없이 펼쳐진 도시의 건물들 뒤로, 잠시 멈춰 선 사람들. 푸른 하늘과 강물이 조화를 이루는 이곳에서, 사람들은 잠시나마 일상의 무게를 내려놓고 자연과 함께 쉼을 찾는다. </t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/1봄_42기_김성근_전자재료공학과.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/1봄_45기_경준하_경영학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/1봄_45기_황서진_컴퓨터정보공학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/1봄_46기_김가영_미디어커뮤니케이션학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/1봄_46기_이재명_미디어커뮤니케이션.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/2여름_42기_김성근_전자재료공학과.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/2여름_42기_변지욱_미디어커뮤니케이션학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/2여름_43기_박하민_건축공학과.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/2여름_43기_신해원_경영학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/2여름_44기_곽철우_정보융합학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/2여름_45기_안예원_국제통상학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/2여름_46기_박예서_전자공학과.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/2여름_46기_배중근_국제학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/2여름_46기_이찬영_국제통상학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/2여름_46기_정성호_동북아문화산업학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/3가을_41기_이민우_화학과.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/3가을_45기_안세은_미디어커뮤니케이션학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/3가을_46기_강민서_전자공학과.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/3가을_46기_박지원_동북아문화산업학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/3가을_46기_방여원_경영학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/3가을_46기_송희수_정보융합학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/3가을_46기_윤영수_미디어커뮤니케이션.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/4겨울_41기_홍자형_스포츠융합과학과.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/4겨울_42기_백채원_영어산업학과.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/4겨울_42기_최승아_컴정공.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/4겨울_44기_이가영_미디어커뮤니케이션학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/4겨울_44기_이아란_정보융합학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/4겨울_46기_김유민_정보융합학부.webp</t>
+  </si>
+  <si>
+    <t>https://www.kapaforever.site/webp/4겨울_46기_유용규_국제학부.webp</t>
   </si>
 </sst>
 </file>
@@ -1175,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243BFB0D-7AC2-2B4E-9AEC-4D6C8DBE03D8}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1221,7 +1218,9 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="20">
-      <c r="A2" s="9"/>
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1244,11 +1243,13 @@
         <v>135</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="40">
-      <c r="A3" s="9"/>
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1271,11 +1272,13 @@
         <v>133</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60">
-      <c r="A4" s="9"/>
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1295,14 +1298,16 @@
         <v>137</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="40">
-      <c r="A5" s="9"/>
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1325,11 +1330,13 @@
         <v>106</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="40">
-      <c r="A6" s="9"/>
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1352,11 +1359,13 @@
         <v>73</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="20">
-      <c r="A7" s="9"/>
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
       <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
@@ -1379,11 +1388,13 @@
         <v>34</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="60">
-      <c r="A8" s="9"/>
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
       <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
@@ -1406,11 +1417,13 @@
         <v>36</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60">
-      <c r="A9" s="9"/>
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1433,11 +1446,13 @@
         <v>60</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="20">
-      <c r="A10" s="9"/>
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
       <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1460,11 +1475,13 @@
         <v>40</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="40">
-      <c r="A11" s="9"/>
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
       <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
@@ -1487,11 +1504,13 @@
         <v>90</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="40">
-      <c r="A12" s="9"/>
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
       <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
@@ -1514,11 +1533,13 @@
         <v>43</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="40">
-      <c r="A13" s="9"/>
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
       <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1541,11 +1562,13 @@
         <v>120</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="40">
-      <c r="A14" s="9"/>
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -1568,11 +1591,13 @@
         <v>69</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="60">
-      <c r="A15" s="9"/>
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
       <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
@@ -1595,11 +1620,13 @@
         <v>79</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="20">
-      <c r="A16" s="9"/>
+      <c r="A16" s="9">
+        <v>15</v>
+      </c>
       <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
@@ -1622,11 +1649,13 @@
         <v>45</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="40">
-      <c r="A17" s="9"/>
+      <c r="A17" s="9">
+        <v>16</v>
+      </c>
       <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
@@ -1649,11 +1678,13 @@
         <v>94</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="20">
-      <c r="A18" s="9"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="40">
+      <c r="A18" s="9">
+        <v>17</v>
+      </c>
       <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
@@ -1676,11 +1707,13 @@
         <v>118</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="20">
-      <c r="A19" s="9"/>
+      <c r="A19" s="9">
+        <v>18</v>
+      </c>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1703,11 +1736,13 @@
         <v>59</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="40">
-      <c r="A20" s="9"/>
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
       <c r="B20" s="5" t="s">
         <v>22</v>
       </c>
@@ -1730,11 +1765,13 @@
         <v>109</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="20">
-      <c r="A21" s="9"/>
+      <c r="A21" s="9">
+        <v>20</v>
+      </c>
       <c r="B21" s="5" t="s">
         <v>22</v>
       </c>
@@ -1757,11 +1794,13 @@
         <v>64</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="40">
-      <c r="A22" s="9"/>
+      <c r="A22" s="9">
+        <v>21</v>
+      </c>
       <c r="B22" s="5" t="s">
         <v>22</v>
       </c>
@@ -1784,11 +1823,13 @@
         <v>42</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="60">
-      <c r="A23" s="9"/>
+      <c r="A23" s="9">
+        <v>22</v>
+      </c>
       <c r="B23" s="5" t="s">
         <v>22</v>
       </c>
@@ -1808,14 +1849,16 @@
         <v>52</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="20">
-      <c r="A24" s="9"/>
+      <c r="A24" s="9">
+        <v>23</v>
+      </c>
       <c r="B24" s="5" t="s">
         <v>23</v>
       </c>
@@ -1838,11 +1881,13 @@
         <v>87</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="40">
-      <c r="A25" s="9"/>
+      <c r="A25" s="9">
+        <v>24</v>
+      </c>
       <c r="B25" s="5" t="s">
         <v>23</v>
       </c>
@@ -1865,11 +1910,13 @@
         <v>114</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="40">
-      <c r="A26" s="9"/>
+      <c r="A26" s="9">
+        <v>25</v>
+      </c>
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
@@ -1892,11 +1939,13 @@
         <v>51</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="20">
-      <c r="A27" s="9"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="40">
+      <c r="A27" s="9">
+        <v>26</v>
+      </c>
       <c r="B27" s="5" t="s">
         <v>23</v>
       </c>
@@ -1919,11 +1968,13 @@
         <v>130</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="60">
-      <c r="A28" s="9"/>
+      <c r="A28" s="9">
+        <v>27</v>
+      </c>
       <c r="B28" s="5" t="s">
         <v>23</v>
       </c>
@@ -1946,11 +1997,13 @@
         <v>102</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="60">
-      <c r="A29" s="9"/>
+      <c r="A29" s="9">
+        <v>28</v>
+      </c>
       <c r="B29" s="5" t="s">
         <v>23</v>
       </c>
@@ -1973,11 +2026,13 @@
         <v>123</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="21" thickBot="1">
-      <c r="A30" s="11"/>
+      <c r="A30" s="9">
+        <v>29</v>
+      </c>
       <c r="B30" s="12" t="s">
         <v>23</v>
       </c>
@@ -2000,7 +2055,7 @@
         <v>98</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:8">

</xml_diff>